<commit_message>
removed unneeded files and moved clarke experiments to separate folder
</commit_message>
<xml_diff>
--- a/completeResults/completeResults_R1_R30_ Copy xlsk.xlsx
+++ b/completeResults/completeResults_R1_R30_ Copy xlsk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Programming\GitHub\Cuckoo-Search-For-CVRP\completeResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A88C8C-FB00-4C44-9AE5-2555A62FAC55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EF50E2-3581-485B-A642-2BB19E7C1EE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-116" yWindow="-116" windowWidth="24917" windowHeight="13513" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16992,7 +16992,7 @@
   <dimension ref="B1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.8" x14ac:dyDescent="0.3"/>

</xml_diff>